<commit_message>
Script for ML added
</commit_message>
<xml_diff>
--- a/HoursSite.xlsx
+++ b/HoursSite.xlsx
@@ -22,16 +22,16 @@
     <t>Plant</t>
   </si>
   <si>
-    <t>553.11</t>
-  </si>
-  <si>
-    <t>875.364</t>
-  </si>
-  <si>
-    <t>312.60200000000003</t>
-  </si>
-  <si>
-    <t>1314.444</t>
+    <t>518.0640000000001</t>
+  </si>
+  <si>
+    <t>946.193</t>
+  </si>
+  <si>
+    <t>325.302</t>
+  </si>
+  <si>
+    <t>1352.583</t>
   </si>
   <si>
     <t>PU1</t>

</xml_diff>